<commit_message>
DOC: Add source in date files
</commit_message>
<xml_diff>
--- a/lifelib/libraries/appliedlife/economic_data/risk_free_202212.xlsx
+++ b/lifelib/libraries/appliedlife/economic_data/risk_free_202212.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27820"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fumito\OneDrive\pyproj\lifelib\lifelib\libraries\appliedlife\economic_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBFCDCF-BED5-4BDE-B476-BBE28E669F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9452ED-6292-4B26-A4E0-2F9FCCB33447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="2" xr2:uid="{3E942908-44BA-4F5B-BF99-964E1945059D}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="3" xr2:uid="{3E942908-44BA-4F5B-BF99-964E1945059D}"/>
   </bookViews>
   <sheets>
     <sheet name="BASE" sheetId="1" r:id="rId1"/>
     <sheet name="UP" sheetId="2" r:id="rId2"/>
     <sheet name="DOWN" sheetId="3" r:id="rId3"/>
+    <sheet name="Notes" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
   <si>
     <t>EUR</t>
   </si>
@@ -50,6 +51,9 @@
   </si>
   <si>
     <t>USD</t>
+  </si>
+  <si>
+    <t>Source: EIOPA - European Insurance and Occupational Pensions Authority, https://eiopa.europa.eu/</t>
   </si>
 </sst>
 </file>
@@ -5582,8 +5586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEC45913-9C73-4D96-B641-9DE2F0EE2185}">
   <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A151" sqref="A151"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L125" sqref="L125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
@@ -8155,4 +8159,24 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E79FA8-B3F8-41D7-9D13-4A195F6E7F90}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>